<commit_message>
cambios en el periodo 3
</commit_message>
<xml_diff>
--- a/Entregables/Informe de avance/Informe de Avance - Periodo 3.xlsx
+++ b/Entregables/Informe de avance/Informe de Avance - Periodo 3.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giuliano\Desktop\Unla-RoyalAcademy\Entregables\Informe de avance\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Cálculos" sheetId="1" r:id="rId1"/>
@@ -280,29 +280,6 @@
   </si>
   <si>
     <t>Desarrollar vista de examen</t>
-  </si>
-  <si>
-    <r>
-      <t>Análisis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>En base al SPI, que da 0,42, y al análisis del periodo anterior, se llega a la conclusión de que el proyecto, si bien sigue retrasado respecto a las metas que debería cumplir, está acercándose al nivel en que debería estar. En el próximo período se buscará seguir implementando medidas que acerquen el SPI al valor ideal de 1.</t>
-    </r>
   </si>
   <si>
     <t>Planned Value</t>
@@ -421,6 +398,29 @@
         <family val="2"/>
       </rPr>
       <t>En base al gráfico, podemos observar que, a diferencia del período numero 2, avanzamos con la mayoría de las actividades planeadas para el tercer período. El AC sigue por debajo del EV.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Análisis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>En base al SPI, que da 0,39, y al análisis del periodo anterior, se llega a la conclusión de que el proyecto, si bien sigue retrasado respecto a las metas que debería cumplir, está acercándose al nivel en que debería estar. En el próximo período se buscará seguir implementando medidas que acerquen el SPI al valor ideal de 1.</t>
     </r>
   </si>
 </sst>
@@ -1649,12 +1649,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1670,50 +1669,17 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1751,6 +1717,51 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1760,22 +1771,11 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1935,22 +1935,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>129</c:v>
+                  <c:v>137</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>181</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193</c:v>
+                  <c:v>233</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>213</c:v>
+                  <c:v>269</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2645,9 +2645,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1007"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="88" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="74">
         <v>8</v>
@@ -2839,7 +2839,7 @@
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="75">
         <v>1</v>
@@ -2886,7 +2886,7 @@
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="84" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="76">
         <v>6</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="6" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="84" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="76">
         <v>6</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="8" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="86" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B8" s="77">
         <v>6</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="10" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B10" s="31">
         <v>6</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="87" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B12" s="31">
         <v>6</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="14" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="85" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="31">
         <v>6</v>
@@ -3387,7 +3387,7 @@
     </row>
     <row r="16" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B16" s="31">
         <v>4</v>
@@ -3434,7 +3434,7 @@
     </row>
     <row r="17" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="85" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B17" s="31">
         <v>4</v>
@@ -3481,7 +3481,7 @@
     </row>
     <row r="18" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="83" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B18" s="31">
         <v>6</v>
@@ -3567,7 +3567,7 @@
     </row>
     <row r="20" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="83" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B20" s="31">
         <v>4</v>
@@ -3610,7 +3610,7 @@
     </row>
     <row r="21" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="83" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B21" s="31">
         <v>4</v>
@@ -3653,7 +3653,7 @@
     </row>
     <row r="22" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="83" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="31">
         <v>2</v>
@@ -3696,7 +3696,7 @@
     </row>
     <row r="23" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B23" s="31">
         <v>6</v>
@@ -3786,7 +3786,7 @@
     </row>
     <row r="25" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="83" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B25" s="31">
         <v>6</v>
@@ -3829,7 +3829,7 @@
     </row>
     <row r="26" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B26" s="31">
         <v>6</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="27" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="83" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="31">
         <v>6</v>
@@ -3977,12 +3977,12 @@
       <c r="D29" s="21"/>
       <c r="E29" s="22"/>
       <c r="F29" s="18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G29" s="21"/>
       <c r="H29" s="22"/>
       <c r="I29" s="18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="J29" s="21"/>
       <c r="K29" s="22"/>
@@ -4000,7 +4000,7 @@
       <c r="W29" s="54"/>
       <c r="X29" s="18">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="Y29" s="18">
         <f t="shared" si="4"/>
@@ -4033,15 +4033,19 @@
       <c r="O30" s="23"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="54"/>
-      <c r="R30" s="23"/>
+      <c r="R30" s="23">
+        <v>8</v>
+      </c>
       <c r="S30" s="17"/>
       <c r="T30" s="54"/>
-      <c r="U30" s="23"/>
+      <c r="U30" s="23">
+        <v>8</v>
+      </c>
       <c r="V30" s="17"/>
       <c r="W30" s="54"/>
       <c r="X30" s="18">
         <f t="shared" ref="X30:Z31" si="6">+L30+I30+F30+C30+U30+R30+O30</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y30" s="18">
         <f t="shared" si="6"/>
@@ -4068,10 +4072,14 @@
       <c r="I31" s="23"/>
       <c r="J31" s="13"/>
       <c r="K31" s="15"/>
-      <c r="L31" s="32"/>
+      <c r="L31" s="32">
+        <v>8</v>
+      </c>
       <c r="M31" s="13"/>
       <c r="N31" s="54"/>
-      <c r="O31" s="23"/>
+      <c r="O31" s="23">
+        <v>8</v>
+      </c>
       <c r="P31" s="17"/>
       <c r="Q31" s="54"/>
       <c r="R31" s="23"/>
@@ -4082,7 +4090,7 @@
       <c r="W31" s="54"/>
       <c r="X31" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y31" s="18">
         <f t="shared" si="6"/>
@@ -4115,15 +4123,19 @@
       <c r="O32" s="23"/>
       <c r="P32" s="17"/>
       <c r="Q32" s="54"/>
-      <c r="R32" s="23"/>
+      <c r="R32" s="23">
+        <v>8</v>
+      </c>
       <c r="S32" s="17"/>
       <c r="T32" s="54"/>
-      <c r="U32" s="23"/>
+      <c r="U32" s="23">
+        <v>8</v>
+      </c>
       <c r="V32" s="17"/>
       <c r="W32" s="54"/>
       <c r="X32" s="18">
         <f t="shared" ref="X32:X33" si="7">+L32+I32+F32+C32+U32+R32+O32</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="Y32" s="18">
         <f t="shared" ref="Y32:Y33" si="8">+M32+J32+G32+D32+V32+S32+P32</f>
@@ -4591,7 +4603,7 @@
       </c>
       <c r="F43" s="69">
         <f t="shared" si="23"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G43" s="68">
         <f t="shared" si="23"/>
@@ -4603,7 +4615,7 @@
       </c>
       <c r="I43" s="67">
         <f t="shared" si="23"/>
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="J43" s="68">
         <f t="shared" si="23"/>
@@ -4615,7 +4627,7 @@
       </c>
       <c r="L43" s="69">
         <f t="shared" si="23"/>
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="M43" s="68">
         <f t="shared" si="23"/>
@@ -4627,7 +4639,7 @@
       </c>
       <c r="O43" s="67">
         <f t="shared" si="23"/>
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P43" s="68">
         <f t="shared" si="23"/>
@@ -4639,7 +4651,7 @@
       </c>
       <c r="R43" s="67">
         <f t="shared" si="23"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="S43" s="68">
         <f t="shared" si="23"/>
@@ -4651,7 +4663,7 @@
       </c>
       <c r="U43" s="69">
         <f t="shared" si="23"/>
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="V43" s="68">
         <f t="shared" si="23"/>
@@ -4663,7 +4675,7 @@
       </c>
       <c r="X43" s="67">
         <f t="shared" si="23"/>
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="Y43" s="68">
         <f t="shared" si="23"/>
@@ -4693,7 +4705,7 @@
       </c>
       <c r="F44" s="38">
         <f t="shared" ref="F44:T44" si="24">+F43+C44</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="G44" s="36">
         <f t="shared" si="24"/>
@@ -4705,7 +4717,7 @@
       </c>
       <c r="I44" s="35">
         <f t="shared" si="24"/>
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="J44" s="36">
         <f t="shared" si="24"/>
@@ -4717,7 +4729,7 @@
       </c>
       <c r="L44" s="38">
         <f t="shared" si="24"/>
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="M44" s="36">
         <f t="shared" si="24"/>
@@ -4729,7 +4741,7 @@
       </c>
       <c r="O44" s="38">
         <f t="shared" si="24"/>
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="P44" s="36">
         <f t="shared" si="24"/>
@@ -4741,7 +4753,7 @@
       </c>
       <c r="R44" s="38">
         <f t="shared" si="24"/>
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="S44" s="36">
         <f t="shared" si="24"/>
@@ -4753,7 +4765,7 @@
       </c>
       <c r="U44" s="38">
         <f>+U43+R44</f>
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="V44" s="36">
         <f>+V43+M44</f>
@@ -4806,14 +4818,14 @@
       </c>
       <c r="B50" s="33">
         <f>I44</f>
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="D50" s="33" t="s">
         <v>28</v>
       </c>
       <c r="E50" s="41">
         <f>+B51-B50</f>
-        <v>-75</v>
+        <v>-83</v>
       </c>
       <c r="F50" s="33" t="s">
         <v>29</v>
@@ -4863,7 +4875,7 @@
       </c>
       <c r="N51" s="33">
         <f>+F44</f>
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O51" s="33">
         <f>+G44</f>
@@ -4887,7 +4899,7 @@
       </c>
       <c r="E52" s="41">
         <f>+B51/B50</f>
-        <v>0.41860465116279072</v>
+        <v>0.39416058394160586</v>
       </c>
       <c r="F52" s="33" t="s">
         <v>37</v>
@@ -4900,7 +4912,7 @@
       </c>
       <c r="N52" s="33">
         <f>+I44</f>
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="O52" s="33">
         <f>+J44</f>
@@ -4930,7 +4942,7 @@
       </c>
       <c r="N53" s="33">
         <f>+L44</f>
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="O53" s="33">
         <f>+M44</f>
@@ -4943,7 +4955,7 @@
     </row>
     <row r="54" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D54" s="33" t="s">
         <v>44</v>
@@ -4966,7 +4978,7 @@
       </c>
       <c r="N54" s="33">
         <f>O44</f>
-        <v>181</v>
+        <v>205</v>
       </c>
       <c r="O54" s="33">
         <f>P44</f>
@@ -4983,7 +4995,7 @@
       </c>
       <c r="E55" s="41">
         <f>+(B46-B51)/(E52*E53)</f>
-        <v>412.08333333333331</v>
+        <v>437.63888888888891</v>
       </c>
       <c r="F55" s="33" t="s">
         <v>49</v>
@@ -4999,7 +5011,7 @@
       </c>
       <c r="N55" s="33">
         <f>R44</f>
-        <v>193</v>
+        <v>233</v>
       </c>
       <c r="O55" s="33">
         <f>S44</f>
@@ -5032,7 +5044,7 @@
       </c>
       <c r="N56" s="33">
         <f>U44</f>
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="O56" s="33">
         <f>V44</f>
@@ -5067,7 +5079,7 @@
       </c>
       <c r="E58" s="41">
         <f>+B52+(B46-B51)/(E53*E52)</f>
-        <v>457.08333333333331</v>
+        <v>482.63888888888891</v>
       </c>
       <c r="F58" s="33" t="s">
         <v>57</v>
@@ -6062,8 +6074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:K24"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:K50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6079,29 +6091,29 @@
   <sheetData>
     <row r="1" spans="1:26" ht="7.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="110"/>
-      <c r="D2" s="110"/>
-      <c r="E2" s="110"/>
-      <c r="F2" s="110"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="110"/>
-      <c r="I2" s="110"/>
-      <c r="J2" s="110"/>
-      <c r="K2" s="110"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
     </row>
     <row r="4" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="119" t="s">
+      <c r="C4" s="109" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="119"/>
-      <c r="E4" s="119"/>
-      <c r="F4" s="119"/>
+      <c r="D4" s="109"/>
+      <c r="E4" s="109"/>
+      <c r="F4" s="109"/>
       <c r="I4" s="33"/>
       <c r="J4" s="33"/>
     </row>
@@ -6109,23 +6121,23 @@
       <c r="B5" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="120">
+      <c r="C5" s="110">
         <v>43749</v>
       </c>
-      <c r="D5" s="120"/>
-      <c r="E5" s="120"/>
-      <c r="F5" s="120"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
     </row>
     <row r="6" spans="1:26" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="111" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="121"/>
-      <c r="E6" s="121"/>
-      <c r="F6" s="121"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="46"/>
@@ -6381,18 +6393,18 @@
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
-      <c r="B22" s="122" t="s">
-        <v>118</v>
-      </c>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="123"/>
-      <c r="H22" s="123"/>
-      <c r="I22" s="123"/>
-      <c r="J22" s="123"/>
-      <c r="K22" s="124"/>
+      <c r="B22" s="112" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="114"/>
       <c r="L22" s="47"/>
       <c r="M22" s="47"/>
       <c r="N22" s="47"/>
@@ -6411,16 +6423,16 @@
     </row>
     <row r="23" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
-      <c r="B23" s="125"/>
-      <c r="C23" s="126"/>
-      <c r="D23" s="126"/>
-      <c r="E23" s="126"/>
-      <c r="F23" s="126"/>
-      <c r="G23" s="126"/>
-      <c r="H23" s="126"/>
-      <c r="I23" s="126"/>
-      <c r="J23" s="126"/>
-      <c r="K23" s="127"/>
+      <c r="B23" s="115"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="116"/>
+      <c r="F23" s="116"/>
+      <c r="G23" s="116"/>
+      <c r="H23" s="116"/>
+      <c r="I23" s="116"/>
+      <c r="J23" s="116"/>
+      <c r="K23" s="117"/>
       <c r="L23" s="47"/>
       <c r="M23" s="47"/>
       <c r="N23" s="47"/>
@@ -6439,16 +6451,16 @@
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="47"/>
-      <c r="B24" s="128"/>
-      <c r="C24" s="129"/>
-      <c r="D24" s="129"/>
-      <c r="E24" s="129"/>
-      <c r="F24" s="129"/>
-      <c r="G24" s="129"/>
-      <c r="H24" s="129"/>
-      <c r="I24" s="129"/>
-      <c r="J24" s="129"/>
-      <c r="K24" s="130"/>
+      <c r="B24" s="118"/>
+      <c r="C24" s="119"/>
+      <c r="D24" s="119"/>
+      <c r="E24" s="119"/>
+      <c r="F24" s="119"/>
+      <c r="G24" s="119"/>
+      <c r="H24" s="119"/>
+      <c r="I24" s="119"/>
+      <c r="J24" s="119"/>
+      <c r="K24" s="120"/>
       <c r="L24" s="47"/>
       <c r="M24" s="47"/>
       <c r="N24" s="47"/>
@@ -6494,36 +6506,36 @@
       <c r="Z25" s="47"/>
     </row>
     <row r="27" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B27" s="110" t="s">
+      <c r="B27" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="C27" s="110"/>
-      <c r="D27" s="110"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="110"/>
-      <c r="G27" s="110"/>
-      <c r="H27" s="110"/>
-      <c r="I27" s="110"/>
-      <c r="J27" s="110"/>
-      <c r="K27" s="110"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="108"/>
+      <c r="F27" s="108"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="108"/>
+      <c r="I27" s="108"/>
+      <c r="J27" s="108"/>
+      <c r="K27" s="108"/>
     </row>
     <row r="32" spans="1:26" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="111" t="s">
+      <c r="B32" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="112"/>
-      <c r="D32" s="111" t="s">
+      <c r="C32" s="122"/>
+      <c r="D32" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="112"/>
-      <c r="F32" s="111" t="s">
+      <c r="E32" s="122"/>
+      <c r="F32" s="121" t="s">
         <v>70</v>
       </c>
-      <c r="G32" s="113"/>
-      <c r="H32" s="113"/>
-      <c r="I32" s="113"/>
-      <c r="J32" s="113"/>
-      <c r="K32" s="112"/>
+      <c r="G32" s="123"/>
+      <c r="H32" s="123"/>
+      <c r="I32" s="123"/>
+      <c r="J32" s="123"/>
+      <c r="K32" s="122"/>
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="48" t="s">
@@ -6533,14 +6545,14 @@
         <f>+Cálculos!B46</f>
         <v>261</v>
       </c>
-      <c r="D33" s="114"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="116"/>
-      <c r="G33" s="117"/>
-      <c r="H33" s="117"/>
-      <c r="I33" s="117"/>
-      <c r="J33" s="117"/>
-      <c r="K33" s="118"/>
+      <c r="D33" s="124"/>
+      <c r="E33" s="125"/>
+      <c r="F33" s="126"/>
+      <c r="G33" s="127"/>
+      <c r="H33" s="127"/>
+      <c r="I33" s="127"/>
+      <c r="J33" s="127"/>
+      <c r="K33" s="128"/>
     </row>
     <row r="34" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="50" t="s">
@@ -6548,18 +6560,18 @@
       </c>
       <c r="C34" s="51">
         <f>+Cálculos!B50</f>
-        <v>129</v>
-      </c>
-      <c r="D34" s="99"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="104" t="s">
-        <v>86</v>
-      </c>
-      <c r="G34" s="105"/>
-      <c r="H34" s="105"/>
-      <c r="I34" s="105"/>
-      <c r="J34" s="105"/>
-      <c r="K34" s="106"/>
+        <v>137</v>
+      </c>
+      <c r="D34" s="100"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="129" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="130"/>
+      <c r="H34" s="130"/>
+      <c r="I34" s="130"/>
+      <c r="J34" s="130"/>
+      <c r="K34" s="131"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="50" t="s">
@@ -6569,16 +6581,16 @@
         <f>+Cálculos!B51</f>
         <v>54</v>
       </c>
-      <c r="D35" s="99"/>
-      <c r="E35" s="100"/>
-      <c r="F35" s="107" t="s">
-        <v>88</v>
-      </c>
-      <c r="G35" s="108"/>
-      <c r="H35" s="108"/>
-      <c r="I35" s="108"/>
-      <c r="J35" s="108"/>
-      <c r="K35" s="109"/>
+      <c r="D35" s="100"/>
+      <c r="E35" s="101"/>
+      <c r="F35" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="132"/>
+      <c r="H35" s="132"/>
+      <c r="I35" s="132"/>
+      <c r="J35" s="132"/>
+      <c r="K35" s="133"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="48" t="s">
@@ -6588,16 +6600,16 @@
         <f>+Cálculos!B52</f>
         <v>45</v>
       </c>
-      <c r="D36" s="99"/>
-      <c r="E36" s="100"/>
-      <c r="F36" s="107" t="s">
-        <v>87</v>
-      </c>
-      <c r="G36" s="108"/>
-      <c r="H36" s="108"/>
-      <c r="I36" s="108"/>
-      <c r="J36" s="108"/>
-      <c r="K36" s="109"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="101"/>
+      <c r="F36" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="132"/>
+      <c r="H36" s="132"/>
+      <c r="I36" s="132"/>
+      <c r="J36" s="132"/>
+      <c r="K36" s="133"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="93" t="s">
@@ -6605,20 +6617,20 @@
       </c>
       <c r="C37" s="49">
         <f>+Cálculos!E50</f>
-        <v>-75</v>
-      </c>
-      <c r="D37" s="99" t="s">
+        <v>-83</v>
+      </c>
+      <c r="D37" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="E37" s="100"/>
-      <c r="F37" s="107" t="s">
-        <v>94</v>
-      </c>
-      <c r="G37" s="134"/>
-      <c r="H37" s="134"/>
-      <c r="I37" s="134"/>
-      <c r="J37" s="134"/>
-      <c r="K37" s="135"/>
+      <c r="E37" s="101"/>
+      <c r="F37" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="98"/>
+      <c r="H37" s="98"/>
+      <c r="I37" s="98"/>
+      <c r="J37" s="98"/>
+      <c r="K37" s="99"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="50" t="s">
@@ -6628,18 +6640,18 @@
         <f>+Cálculos!E51</f>
         <v>9</v>
       </c>
-      <c r="D38" s="99" t="s">
+      <c r="D38" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="E38" s="138"/>
-      <c r="F38" s="101" t="s">
-        <v>89</v>
-      </c>
-      <c r="G38" s="139"/>
-      <c r="H38" s="139"/>
-      <c r="I38" s="139"/>
-      <c r="J38" s="139"/>
-      <c r="K38" s="140"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="102" t="s">
+        <v>88</v>
+      </c>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106"/>
+      <c r="K38" s="107"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="50" t="s">
@@ -6647,20 +6659,20 @@
       </c>
       <c r="C39" s="51">
         <f>+Cálculos!E52</f>
-        <v>0.41860465116279072</v>
-      </c>
-      <c r="D39" s="99" t="s">
+        <v>0.39416058394160586</v>
+      </c>
+      <c r="D39" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E39" s="100"/>
-      <c r="F39" s="101" t="s">
-        <v>95</v>
-      </c>
-      <c r="G39" s="102"/>
-      <c r="H39" s="102"/>
-      <c r="I39" s="102"/>
-      <c r="J39" s="102"/>
-      <c r="K39" s="103"/>
+      <c r="E39" s="101"/>
+      <c r="F39" s="102" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="103"/>
+      <c r="H39" s="103"/>
+      <c r="I39" s="103"/>
+      <c r="J39" s="103"/>
+      <c r="K39" s="104"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B40" s="50" t="s">
@@ -6670,18 +6682,18 @@
         <f>+Cálculos!E53</f>
         <v>1.2</v>
       </c>
-      <c r="D40" s="99" t="s">
+      <c r="D40" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="100"/>
-      <c r="F40" s="101" t="s">
-        <v>90</v>
-      </c>
-      <c r="G40" s="102"/>
-      <c r="H40" s="102"/>
-      <c r="I40" s="102"/>
-      <c r="J40" s="102"/>
-      <c r="K40" s="103"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="102" t="s">
+        <v>89</v>
+      </c>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+      <c r="K40" s="104"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="50" t="s">
@@ -6691,18 +6703,18 @@
         <f>+Cálculos!E54</f>
         <v>207</v>
       </c>
-      <c r="D41" s="99" t="s">
+      <c r="D41" s="100" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="100"/>
-      <c r="F41" s="101" t="s">
-        <v>98</v>
-      </c>
-      <c r="G41" s="102"/>
-      <c r="H41" s="102"/>
-      <c r="I41" s="102"/>
-      <c r="J41" s="102"/>
-      <c r="K41" s="103"/>
+      <c r="E41" s="101"/>
+      <c r="F41" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="G41" s="103"/>
+      <c r="H41" s="103"/>
+      <c r="I41" s="103"/>
+      <c r="J41" s="103"/>
+      <c r="K41" s="104"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="50" t="s">
@@ -6710,20 +6722,20 @@
       </c>
       <c r="C42" s="51">
         <f>+Cálculos!E55</f>
-        <v>412.08333333333331</v>
-      </c>
-      <c r="D42" s="99" t="s">
+        <v>437.63888888888891</v>
+      </c>
+      <c r="D42" s="100" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="100"/>
-      <c r="F42" s="101" t="s">
-        <v>99</v>
-      </c>
-      <c r="G42" s="102"/>
-      <c r="H42" s="102"/>
-      <c r="I42" s="102"/>
-      <c r="J42" s="102"/>
-      <c r="K42" s="103"/>
+      <c r="E42" s="101"/>
+      <c r="F42" s="102" t="s">
+        <v>98</v>
+      </c>
+      <c r="G42" s="103"/>
+      <c r="H42" s="103"/>
+      <c r="I42" s="103"/>
+      <c r="J42" s="103"/>
+      <c r="K42" s="104"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="50" t="s">
@@ -6733,18 +6745,18 @@
         <f>+Cálculos!E56</f>
         <v>252</v>
       </c>
-      <c r="D43" s="99" t="s">
+      <c r="D43" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="100"/>
-      <c r="F43" s="101" t="s">
-        <v>91</v>
-      </c>
-      <c r="G43" s="102"/>
-      <c r="H43" s="102"/>
-      <c r="I43" s="102"/>
-      <c r="J43" s="102"/>
-      <c r="K43" s="103"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="102" t="s">
+        <v>90</v>
+      </c>
+      <c r="G43" s="103"/>
+      <c r="H43" s="103"/>
+      <c r="I43" s="103"/>
+      <c r="J43" s="103"/>
+      <c r="K43" s="104"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="50" t="s">
@@ -6754,18 +6766,18 @@
         <f>+Cálculos!E57</f>
         <v>217.5</v>
       </c>
-      <c r="D44" s="99" t="s">
+      <c r="D44" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="E44" s="100"/>
-      <c r="F44" s="101" t="s">
-        <v>92</v>
-      </c>
-      <c r="G44" s="102"/>
-      <c r="H44" s="102"/>
-      <c r="I44" s="102"/>
-      <c r="J44" s="102"/>
-      <c r="K44" s="103"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="102" t="s">
+        <v>91</v>
+      </c>
+      <c r="G44" s="103"/>
+      <c r="H44" s="103"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="103"/>
+      <c r="K44" s="104"/>
     </row>
     <row r="45" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="50" t="s">
@@ -6773,20 +6785,20 @@
       </c>
       <c r="C45" s="51">
         <f>+Cálculos!E58</f>
-        <v>457.08333333333331</v>
-      </c>
-      <c r="D45" s="99" t="s">
+        <v>482.63888888888891</v>
+      </c>
+      <c r="D45" s="100" t="s">
         <v>57</v>
       </c>
-      <c r="E45" s="100"/>
-      <c r="F45" s="101" t="s">
-        <v>93</v>
-      </c>
-      <c r="G45" s="102"/>
-      <c r="H45" s="102"/>
-      <c r="I45" s="102"/>
-      <c r="J45" s="102"/>
-      <c r="K45" s="103"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="102" t="s">
+        <v>92</v>
+      </c>
+      <c r="G45" s="103"/>
+      <c r="H45" s="103"/>
+      <c r="I45" s="103"/>
+      <c r="J45" s="103"/>
+      <c r="K45" s="104"/>
     </row>
     <row r="46" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B46" s="52" t="s">
@@ -6796,34 +6808,34 @@
         <f>+Cálculos!E59</f>
         <v>0.95833333333333337</v>
       </c>
-      <c r="D46" s="136" t="s">
+      <c r="D46" s="139" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="137"/>
-      <c r="F46" s="131" t="s">
-        <v>97</v>
-      </c>
-      <c r="G46" s="132"/>
-      <c r="H46" s="132"/>
-      <c r="I46" s="132"/>
-      <c r="J46" s="132"/>
-      <c r="K46" s="133"/>
+      <c r="E46" s="140"/>
+      <c r="F46" s="136" t="s">
+        <v>96</v>
+      </c>
+      <c r="G46" s="137"/>
+      <c r="H46" s="137"/>
+      <c r="I46" s="137"/>
+      <c r="J46" s="137"/>
+      <c r="K46" s="138"/>
     </row>
     <row r="47" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="47"/>
-      <c r="B48" s="122" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="123"/>
-      <c r="D48" s="123"/>
-      <c r="E48" s="123"/>
-      <c r="F48" s="123"/>
-      <c r="G48" s="123"/>
-      <c r="H48" s="123"/>
-      <c r="I48" s="123"/>
-      <c r="J48" s="123"/>
-      <c r="K48" s="124"/>
+      <c r="B48" s="112" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="113"/>
+      <c r="D48" s="113"/>
+      <c r="E48" s="113"/>
+      <c r="F48" s="113"/>
+      <c r="G48" s="113"/>
+      <c r="H48" s="113"/>
+      <c r="I48" s="113"/>
+      <c r="J48" s="113"/>
+      <c r="K48" s="114"/>
       <c r="L48" s="47"/>
       <c r="M48" s="47"/>
       <c r="N48" s="47"/>
@@ -6842,16 +6854,16 @@
     </row>
     <row r="49" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47"/>
-      <c r="B49" s="125"/>
-      <c r="C49" s="126"/>
-      <c r="D49" s="126"/>
-      <c r="E49" s="126"/>
-      <c r="F49" s="126"/>
-      <c r="G49" s="126"/>
-      <c r="H49" s="126"/>
-      <c r="I49" s="126"/>
-      <c r="J49" s="126"/>
-      <c r="K49" s="127"/>
+      <c r="B49" s="115"/>
+      <c r="C49" s="116"/>
+      <c r="D49" s="116"/>
+      <c r="E49" s="116"/>
+      <c r="F49" s="116"/>
+      <c r="G49" s="116"/>
+      <c r="H49" s="116"/>
+      <c r="I49" s="116"/>
+      <c r="J49" s="116"/>
+      <c r="K49" s="117"/>
       <c r="L49" s="47"/>
       <c r="M49" s="47"/>
       <c r="N49" s="47"/>
@@ -6870,16 +6882,16 @@
     </row>
     <row r="50" spans="1:26" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="47"/>
-      <c r="B50" s="128"/>
-      <c r="C50" s="129"/>
-      <c r="D50" s="129"/>
-      <c r="E50" s="129"/>
-      <c r="F50" s="129"/>
-      <c r="G50" s="129"/>
-      <c r="H50" s="129"/>
-      <c r="I50" s="129"/>
-      <c r="J50" s="129"/>
-      <c r="K50" s="130"/>
+      <c r="B50" s="118"/>
+      <c r="C50" s="119"/>
+      <c r="D50" s="119"/>
+      <c r="E50" s="119"/>
+      <c r="F50" s="119"/>
+      <c r="G50" s="119"/>
+      <c r="H50" s="119"/>
+      <c r="I50" s="119"/>
+      <c r="J50" s="119"/>
+      <c r="K50" s="120"/>
       <c r="L50" s="47"/>
       <c r="M50" s="47"/>
       <c r="N50" s="47"/>
@@ -6926,16 +6938,16 @@
     </row>
     <row r="52" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="53" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I53" s="97"/>
-      <c r="J53" s="97"/>
-      <c r="K53" s="97"/>
+      <c r="I53" s="134"/>
+      <c r="J53" s="134"/>
+      <c r="K53" s="134"/>
     </row>
     <row r="54" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I54" s="98" t="s">
+      <c r="I54" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="J54" s="98"/>
-      <c r="K54" s="98"/>
+      <c r="J54" s="135"/>
+      <c r="K54" s="135"/>
     </row>
     <row r="55" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7885,6 +7897,32 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:K41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:K42"/>
+    <mergeCell ref="B48:K50"/>
+    <mergeCell ref="F46:K46"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:K34"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:K35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:K36"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="B22:K24"/>
     <mergeCell ref="F37:K37"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="F45:K45"/>
@@ -7899,32 +7937,6 @@
     <mergeCell ref="F38:K38"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="F40:K40"/>
-    <mergeCell ref="B2:K2"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="B22:K24"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="F34:K34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:K35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F36:K36"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:K41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:K42"/>
-    <mergeCell ref="B48:K50"/>
-    <mergeCell ref="F46:K46"/>
-    <mergeCell ref="D46:E46"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>